<commit_message>
Arreglo Carpeta Trabajo, HU, IREB
</commit_message>
<xml_diff>
--- a/Biblioteca de Trabajo/1. ELICITACIÓN/1.4 Historias de Usuario/HU_V1.0.0.xlsx
+++ b/Biblioteca de Trabajo/1. ELICITACIÓN/1.4 Historias de Usuario/HU_V1.0.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESPE\Analisis&amp;Diseño\27837_G1_ADS\PREGAME\1. ELICITACIÓN\1.3 Historias de Usuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abner\Desktop\Github\27837_G1_ADS\Biblioteca de Trabajo\1. ELICITACIÓN\1.4 Historias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333417B5-0D16-43F6-9B32-AE144620B4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8577EE77-5EFA-42E5-B073-517DD0482A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,20 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="zqQjEeih5K8NWczfqLGaZHv5HRqGCKJmm/RpsPz/4HQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="dyizzRkkwcblVR9ZrNviAim9gEVYFdPqGnZTU6oXUKU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -87,16 +89,70 @@
     <t xml:space="preserve">NOMBRE DE HISTORIA </t>
   </si>
   <si>
+    <t>RF01</t>
+  </si>
+  <si>
+    <t>Los usuarios no pueden registrar ni controlar sus medicamentos.</t>
+  </si>
+  <si>
+    <t>Permitir registrar, editar y eliminar medicamentos.</t>
+  </si>
+  <si>
+    <t>Para que los adultos mayores puedan administrar su medicación y mantener un historial organizado.</t>
+  </si>
+  <si>
     <t>Usuario adulto mayor / Cuidador</t>
+  </si>
+  <si>
+    <t>Ingresar nombre, dosis, frecuencia, duración, notas y configurar recordatorios e íconos.</t>
   </si>
   <si>
     <t>Marcelo Acuña</t>
   </si>
   <si>
+    <t>Alta</t>
+  </si>
+  <si>
     <t>No iniciado</t>
   </si>
   <si>
-    <t>RF06</t>
+    <t>Se valida que los campos sean obligatorios y se confirme el mensaje “Medicamento guardado exitosamente”.</t>
+  </si>
+  <si>
+    <t>Requisito base del sistema.</t>
+  </si>
+  <si>
+    <t>Gestión de medicamentos</t>
+  </si>
+  <si>
+    <t>RF02</t>
+  </si>
+  <si>
+    <t>El usuario olvida tomar la medicación a tiempo.</t>
+  </si>
+  <si>
+    <t>Generar recordatorios automáticos con alertas visuales, sonoras y por vibración.</t>
+  </si>
+  <si>
+    <t>Para garantizar la adherencia al tratamiento médico.</t>
+  </si>
+  <si>
+    <t>Usuario adulto mayor</t>
+  </si>
+  <si>
+    <t>El sistema genera una alerta a la hora programada; el usuario marca como tomada, pospone o indica omisión.</t>
+  </si>
+  <si>
+    <t>Se comprueba que la notificación aparezca incluso con la pantalla bloqueada y persista hasta acción del usuario.</t>
+  </si>
+  <si>
+    <t>Vital para la adherencia al tratamiento.</t>
+  </si>
+  <si>
+    <t>Recordatorios de medicación</t>
+  </si>
+  <si>
+    <t>RF03</t>
   </si>
   <si>
     <t>No hay un registro consolidado del historial de tomas.</t>
@@ -129,7 +185,7 @@
     <t>Informes de historial de medicación</t>
   </si>
   <si>
-    <t>RF07</t>
+    <t>RF04</t>
   </si>
   <si>
     <t>El usuario no tiene seguimiento de síntomas o efectos secundarios.</t>
@@ -156,7 +212,7 @@
     <t>Seguimiento de síntomas</t>
   </si>
   <si>
-    <t>RF08</t>
+    <t>RF05</t>
   </si>
   <si>
     <t>El cuidador gestiona varios pacientes y no puede separar información.</t>
@@ -685,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -765,40 +821,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -811,11 +835,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,21 +869,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,7 +943,7 @@
     <xdr:ext cx="1066800" cy="1162050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.jpg">
+        <xdr:cNvPr id="2" name="image2.jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
@@ -948,7 +977,7 @@
     <xdr:ext cx="1095375" cy="1162050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image2.jpg">
+        <xdr:cNvPr id="3" name="image1.jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
@@ -1176,10 +1205,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z972"/>
+  <dimension ref="A1:Z974"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1368,46 +1397,46 @@
     <row r="6" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>45870</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="M6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="6">
-        <v>3</v>
-      </c>
-      <c r="J6" s="7">
-        <v>45984</v>
-      </c>
-      <c r="K6" s="8" t="s">
+      <c r="N6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="9" t="s">
+      <c r="O6" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1421,49 +1450,49 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>45870</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="6">
-        <v>3</v>
-      </c>
-      <c r="J7" s="7">
-        <v>45985</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="O7" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1477,40 +1506,40 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="6">
+        <v>3</v>
+      </c>
+      <c r="J8" s="7">
+        <v>45870</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="6">
-        <v>4</v>
-      </c>
-      <c r="J8" s="7">
-        <v>45986</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="L8" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>44</v>
@@ -1533,22 +1562,50 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="B9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="6">
+        <v>3</v>
+      </c>
+      <c r="J9" s="7">
+        <v>45870</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1561,22 +1618,50 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="6">
+        <v>4</v>
+      </c>
+      <c r="J10" s="7">
+        <v>45870</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1589,7 +1674,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1617,7 +1702,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1647,6 +1732,20 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1661,6 +1760,20 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1675,6 +1788,20 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1689,6 +1816,20 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -7077,22 +7218,76 @@
       <c r="Y208" s="1"/>
       <c r="Z208" s="1"/>
     </row>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="2"/>
+      <c r="J209" s="2"/>
+      <c r="K209" s="3"/>
+      <c r="L209" s="2"/>
+      <c r="M209" s="1"/>
+      <c r="N209" s="1"/>
+      <c r="O209" s="1"/>
+      <c r="P209" s="1"/>
+      <c r="Q209" s="1"/>
+      <c r="R209" s="1"/>
+      <c r="S209" s="1"/>
+      <c r="T209" s="1"/>
+      <c r="U209" s="1"/>
+      <c r="V209" s="1"/>
+      <c r="W209" s="1"/>
+      <c r="X209" s="1"/>
+      <c r="Y209" s="1"/>
+      <c r="Z209" s="1"/>
+    </row>
+    <row r="210" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1"/>
+      <c r="F210" s="1"/>
+      <c r="G210" s="1"/>
+      <c r="H210" s="1"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+      <c r="K210" s="3"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="1"/>
+      <c r="N210" s="1"/>
+      <c r="O210" s="1"/>
+      <c r="P210" s="1"/>
+      <c r="Q210" s="1"/>
+      <c r="R210" s="1"/>
+      <c r="S210" s="1"/>
+      <c r="T210" s="1"/>
+      <c r="U210" s="1"/>
+      <c r="V210" s="1"/>
+      <c r="W210" s="1"/>
+      <c r="X210" s="1"/>
+      <c r="Y210" s="1"/>
+      <c r="Z210" s="1"/>
+    </row>
+    <row r="211" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7841,21 +8036,13 @@
     <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:O3"/>
   </mergeCells>
-  <conditionalFormatting sqref="L13:L16 L6:L8">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFFFFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="L9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -7865,8 +8052,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L10">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:L8" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:L10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -7883,9 +8080,7 @@
   </sheetPr>
   <dimension ref="A2:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7911,8 +8106,8 @@
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="69" t="s">
-        <v>47</v>
+      <c r="B6" s="37" t="s">
+        <v>65</v>
       </c>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
@@ -7981,12 +8176,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="52" t="s">
-        <v>48</v>
+      <c r="E9" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="F9" s="36"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="52" t="s">
+      <c r="H9" s="38" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="36"/>
@@ -8002,17 +8197,17 @@
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="24" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="70" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,5,0)</f>
-        <v>Cuidador / Profesional de salud</v>
-      </c>
-      <c r="F10" s="71"/>
+      <c r="E10" s="39" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,5,0)</f>
+        <v>Usuario adulto mayor</v>
+      </c>
+      <c r="F10" s="36"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="53" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,11,0)</f>
+      <c r="H10" s="39" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,11,0)</f>
         <v>No iniciado</v>
       </c>
       <c r="I10" s="36"/>
@@ -8057,16 +8252,16 @@
       <c r="A12" s="12"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="38" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="52" t="s">
-        <v>50</v>
+      <c r="H12" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="I12" s="36"/>
       <c r="J12" s="26"/>
@@ -8091,19 +8286,19 @@
       <c r="A13" s="12"/>
       <c r="B13" s="19"/>
       <c r="C13" s="29">
-        <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O8,8,0)</f>
-        <v>3</v>
+        <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O10,8,0)</f>
+        <v>5</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="53" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,10,0)</f>
-        <v>Media</v>
+      <c r="E13" s="39" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,10,0)</f>
+        <v>Alta</v>
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="53" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,7,0)</f>
-        <v>Abner Arboleda</v>
+      <c r="H13" s="39" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,7,0)</f>
+        <v>Marcelo Acuña</v>
       </c>
       <c r="I13" s="36"/>
       <c r="J13" s="26"/>
@@ -8155,34 +8350,34 @@
     <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="43" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,3,0)</f>
-        <v>Registrar eventos (tomado, omitido, pospuesto) y generar informes.</v>
-      </c>
-      <c r="E15" s="38"/>
+      <c r="C15" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="55" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,3,0)</f>
+        <v>Generar recordatorios automáticos con alertas visuales, sonoras y por vibración.</v>
+      </c>
+      <c r="E15" s="44"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="43" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,4,0)</f>
-        <v>Para que el usuario o cuidador puedan visualizar y compartir el historial.</v>
-      </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="38"/>
+      <c r="G15" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="55" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,4,0)</f>
+        <v>Para garantizar la adherencia al tratamiento médico.</v>
+      </c>
+      <c r="I15" s="51"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="M15" s="60" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,6,0)</f>
-        <v>Generar reportes PDF con fecha, hora y motivo de cada acción.</v>
-      </c>
-      <c r="N15" s="44"/>
-      <c r="O15" s="45"/>
+      <c r="L15" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="56" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,6,0)</f>
+        <v>El sistema genera una alerta a la hora programada; el usuario marca como tomada, pospone o indica omisión.</v>
+      </c>
+      <c r="N15" s="51"/>
+      <c r="O15" s="44"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
@@ -8198,19 +8393,19 @@
     <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="19"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="40"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="49"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="48"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="49"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
@@ -8226,19 +8421,19 @@
     <row r="17" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="19"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="30"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="46"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="51"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="46"/>
       <c r="P17" s="23"/>
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
@@ -8281,42 +8476,42 @@
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="61" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,14,0)</f>
-        <v>Informes de historial de medicación</v>
-      </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="63"/>
+      <c r="C19" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="57" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,14,0)</f>
+        <v>Recordatorios de medicación</v>
+      </c>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="59"/>
       <c r="P19" s="23"/>
       <c r="Q19" s="12"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="66"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="62"/>
       <c r="P20" s="23"/>
       <c r="Q20" s="12"/>
     </row>
@@ -8341,29 +8536,29 @@
     <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="19"/>
-      <c r="C22" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="68" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,12,0)</f>
-        <v>Se genera un PDF y se verifica que todos los eventos estén listados correctamente.</v>
-      </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="45"/>
+      <c r="C22" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="50" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,12,0)</f>
+        <v>Se comprueba que la notificación aparezca incluso con la pantalla bloqueada y persista hasta acción del usuario.</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="44"/>
       <c r="I22" s="22"/>
-      <c r="J22" s="37" t="s">
+      <c r="J22" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="38"/>
-      <c r="L22" s="43" t="str">
-        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O8,13,0)</f>
-        <v>Compatible con exportación a Excel.</v>
-      </c>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="45"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="54" t="str">
+        <f>VLOOKUP(C10,'Formato descripción HU'!B6:O10,13,0)</f>
+        <v>Vital para la adherencia al tratamiento.</v>
+      </c>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="23"/>
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
@@ -8379,19 +8574,19 @@
     <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="19"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="49"/>
       <c r="I23" s="22"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="49"/>
       <c r="P23" s="23"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
@@ -8407,19 +8602,19 @@
     <row r="24" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="19"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="51"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="46"/>
       <c r="I24" s="22"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="51"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="46"/>
       <c r="P24" s="23"/>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
@@ -9978,15 +10173,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="C22:D24"/>
-    <mergeCell ref="E22:H24"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="J22:K24"/>
     <mergeCell ref="L22:O24"/>
     <mergeCell ref="H12:I12"/>
@@ -9999,6 +10185,15 @@
     <mergeCell ref="E19:O20"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="C22:D24"/>
+    <mergeCell ref="E22:H24"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -10029,7 +10224,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>'Formato descripción HU'!$B$6:$B$8</xm:f>
+            <xm:f>'Formato descripción HU'!$B$6:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>C10:C11</xm:sqref>
         </x14:dataValidation>

</xml_diff>